<commit_message>
Implement new industrial process emissions input data and policy levers.  Update policy scenarios and WebAppData accordingly. (#20)
</commit_message>
<xml_diff>
--- a/InputData/cost-outputs/CFQS/Cash Flow Quantization Size.xlsx
+++ b/InputData/cost-outputs/CFQS/Cash Flow Quantization Size.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipN\InputData\cost-outputs\CFQS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="14100"/>
   </bookViews>
@@ -76,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,7 +526,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>100000</v>
+        <v>400000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>